<commit_message>
this is the final power bi training assessments
</commit_message>
<xml_diff>
--- a/01_Python/12_Mic_Forms/categorized_training_needsv2.xlsx
+++ b/01_Python/12_Mic_Forms/categorized_training_needsv2.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BQ2"/>
+  <dimension ref="A1:BQ3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -953,6 +953,175 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45192.45601851852</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45192.45664351852</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Hossam.Ibrahim</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Hossam Tabana</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Geospatial Maps</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Sometimes</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Yes, simple calculations</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Beginner level</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Basic transformations only</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>Yes, basic automation</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>Occasionally</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Very Important</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Yes, as static files</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>Occasionally</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>Yes, it's essential</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>Not concerned</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>Just exploring</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>Yes, basic trend lines</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>Definitely</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr"/>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>I know what it is but haven't used it</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr"/>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>Possibly</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr"/>
+      <c r="BJ3" t="inlineStr"/>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>Yes, to multiple formats</t>
+        </is>
+      </c>
+      <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
+      <c r="BN3" t="inlineStr">
+        <is>
+          <t>Using Power BI workspaces</t>
+        </is>
+      </c>
+      <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>Medium Training</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>